<commit_message>
add graph for resnet 101 10gbps, in rack, uneven, striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_uneven_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_uneven_striping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -261,19 +258,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0103</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2617</c:v>
+                    <c:v>0.2637</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.543</c:v>
+                    <c:v>3.508</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.6986</c:v>
+                    <c:v>2.7845</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6296</c:v>
+                    <c:v>1.4554</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0013</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.8581</c:v>
+                    <c:v>0.8217</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>5.5888</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4518</c:v>
+                    <c:v>0.7329</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5538</c:v>
+                    <c:v>0.2355</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -347,19 +344,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.2381</c:v>
+                  <c:v>16.8057</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>39.0169</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.3669</c:v>
+                  <c:v>37.0194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.7375</c:v>
+                  <c:v>43.4378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,7 +405,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1321</c:v>
+                    <c:v>0.5806</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0</c:v>
@@ -417,10 +414,10 @@
                     <c:v>7.0322</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.215</c:v>
+                    <c:v>6.7497</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.6037</c:v>
+                    <c:v>3.8679</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,7 +429,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1496</c:v>
+                    <c:v>0.5234</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0</c:v>
@@ -441,10 +438,10 @@
                     <c:v>11.3765</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.4233</c:v>
+                    <c:v>2.6385</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.1419</c:v>
+                    <c:v>2.9095</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -494,7 +491,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.1718</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -503,10 +500,10 @@
                   <c:v>29.5048</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.7402</c:v>
+                  <c:v>27.2869</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.2816</c:v>
+                  <c:v>37.7758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0554</c:v>
+                    <c:v>0.2758</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6818</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.0158</c:v>
+                    <c:v>10.3392</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>13.5675</c:v>
+                    <c:v>5.0261</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9889</c:v>
+                    <c:v>6.1887</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -579,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0567</c:v>
+                    <c:v>0.0925</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.7947</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>17.6853</c:v>
+                    <c:v>16.3748</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.7147</c:v>
+                    <c:v>2.9021</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.4946</c:v>
+                    <c:v>4.3337</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -641,19 +638,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0917</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.192</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.406</c:v>
+                  <c:v>20.079</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.6884</c:v>
+                  <c:v>14.3511</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.6941</c:v>
+                  <c:v>29.5063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.3294</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>1.9749</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.4734</c:v>
+                    <c:v>11.4017</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>15.063</c:v>
+                    <c:v>19.7157</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0788</c:v>
+                    <c:v>7.0031</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -726,19 +723,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.109</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>1.4681</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>17.539</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6026</c:v>
+                    <c:v>2.9286</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0718</c:v>
+                    <c:v>1.0716</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -788,19 +785,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.3316</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.2441</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20.9594</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.174</c:v>
+                  <c:v>14.4742</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.4486</c:v>
+                  <c:v>30.1845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2115197568"/>
-        <c:axId val="-2116017200"/>
+        <c:axId val="-2093661312"/>
+        <c:axId val="-2093653248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2115197568"/>
+        <c:axId val="-2093661312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116017200"/>
+        <c:crossAx val="-2093653248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2116017200"/>
+        <c:axId val="-2093653248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115197568"/>
+        <c:crossAx val="-2093661312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1073</c:v>
+                    <c:v>1.3125</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0104</c:v>
+                    <c:v>0.0292</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3122</c:v>
+                    <c:v>0.9778</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7372</c:v>
+                    <c:v>0.445</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.5275</c:v>
+                    <c:v>0.2828</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0141</c:v>
+                    <c:v>0.0104</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0592</c:v>
+                    <c:v>0.188</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3112</c:v>
+                    <c:v>0.1492</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1379,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3.8346</c:v>
+                  <c:v>10.9074</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.9838</c:v>
+                  <c:v>27.0252</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.9732</c:v>
+                  <c:v>37.5782</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.3864</c:v>
+                  <c:v>43.5479</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.4701</c:v>
+                  <c:v>46.825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0711</c:v>
+                    <c:v>1.0181</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0435</c:v>
+                    <c:v>0.068</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0042</c:v>
+                    <c:v>1.2954</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2445</c:v>
+                    <c:v>0.4484</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0609</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0148</c:v>
+                    <c:v>0.2003</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0194</c:v>
+                    <c:v>0.0281</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3983</c:v>
+                    <c:v>0.1845</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3212</c:v>
+                    <c:v>0.1063</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.6665</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.3066</c:v>
+                  <c:v>15.2135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.0388</c:v>
+                  <c:v>33.5407</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.4919</c:v>
+                  <c:v>41.7519</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.2404</c:v>
+                  <c:v>45.8726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0554</c:v>
+                    <c:v>0.0836</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4131</c:v>
+                    <c:v>0.9549</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0294</c:v>
+                    <c:v>0.2003</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.8938</c:v>
+                    <c:v>0.1015</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2844</c:v>
+                    <c:v>2.2766</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1611,19 +1608,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.126</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1407</c:v>
+                    <c:v>0.2952</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0638</c:v>
+                    <c:v>0.1996</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.7881</c:v>
+                    <c:v>0.9853</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2095</c:v>
+                    <c:v>1.9031</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1673,19 +1670,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0224</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-25.8263</c:v>
+                  <c:v>0.8075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2623</c:v>
+                  <c:v>14.321</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.0164</c:v>
+                  <c:v>28.4768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.5203</c:v>
+                  <c:v>39.1733</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,19 +1731,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.2617</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0134</c:v>
+                    <c:v>1.2133</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2344</c:v>
+                    <c:v>0.144</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.3728</c:v>
+                    <c:v>2.1941</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6405</c:v>
+                    <c:v>1.8188</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1758,19 +1755,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.5973</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0394</c:v>
+                    <c:v>0.8722</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0172</c:v>
+                    <c:v>0.2185</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.8101</c:v>
+                    <c:v>0.5356</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3914</c:v>
+                    <c:v>0.9528</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1820,19 +1817,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.1591</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2289</c:v>
+                  <c:v>0.0161</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8248</c:v>
+                  <c:v>15.3652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.5814</c:v>
+                  <c:v>31.9738</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.4379</c:v>
+                  <c:v>41.106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2066607664"/>
-        <c:axId val="-2115276800"/>
+        <c:axId val="-2093524384"/>
+        <c:axId val="-2093518128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2066607664"/>
+        <c:axId val="-2093524384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115276800"/>
+        <c:crossAx val="-2093518128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2115276800"/>
+        <c:axId val="-2093518128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066607664"/>
+        <c:crossAx val="-2093524384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1073</c:v>
+                    <c:v>1.3125</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2618</c:v>
+                    <c:v>0.2553</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.3452</c:v>
+                    <c:v>3.6374</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.9843</c:v>
+                    <c:v>2.0847</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8458</c:v>
+                    <c:v>0.4473</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.5275</c:v>
+                    <c:v>0.2828</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.8388</c:v>
+                    <c:v>0.8094</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5889</c:v>
+                    <c:v>5.5932</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.395</c:v>
+                    <c:v>3.1308</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2715</c:v>
+                    <c:v>2.6129</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3.8346</c:v>
+                  <c:v>10.9074</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.2218</c:v>
+                  <c:v>43.8393</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.9902</c:v>
+                  <c:v>76.5995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81.6616</c:v>
+                  <c:v>80.9331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.1277</c:v>
+                  <c:v>91.4678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0711</c:v>
+                    <c:v>1.0181</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0435</c:v>
+                    <c:v>0.068</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.0129</c:v>
+                    <c:v>7.0041</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.9886</c:v>
+                    <c:v>8.6196</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0382</c:v>
+                    <c:v>3.2631</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0609</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0148</c:v>
+                    <c:v>0.2003</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.3764</c:v>
+                    <c:v>11.3765</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.3269</c:v>
+                    <c:v>1.1789</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6744</c:v>
+                    <c:v>2.7075</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.6665</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.3066</c:v>
+                  <c:v>15.2135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.5435</c:v>
+                  <c:v>63.0455</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64.3435</c:v>
+                  <c:v>67.2995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.2291</c:v>
+                  <c:v>83.5762</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0554</c:v>
+                    <c:v>0.0836</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4131</c:v>
+                    <c:v>0.9549</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.0102</c:v>
+                    <c:v>10.3108</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.9907</c:v>
+                    <c:v>8.8292</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6915</c:v>
+                    <c:v>1.5918</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2643,19 +2640,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.126</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1407</c:v>
+                    <c:v>0.2952</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>17.6909</c:v>
+                    <c:v>16.4244</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.1748</c:v>
+                    <c:v>4.2924</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8051</c:v>
+                    <c:v>0.8103</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2705,19 +2702,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0224</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-25.8263</c:v>
+                  <c:v>0.8075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.6977</c:v>
+                  <c:v>34.4283</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.7456</c:v>
+                  <c:v>45.9533</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.3836</c:v>
+                  <c:v>69.575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2763,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.2617</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0134</c:v>
+                    <c:v>1.2133</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.4563</c:v>
+                    <c:v>11.3246</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.6696</c:v>
+                    <c:v>11.2408</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.0217</c:v>
+                    <c:v>2.2287</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2790,19 +2787,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.5973</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0394</c:v>
+                    <c:v>0.8722</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>17.5532</c:v>
+                    <c:v>17.6161</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.9104</c:v>
+                    <c:v>8.1856</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.5377</c:v>
+                    <c:v>0.8344</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2852,19 +2849,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.1591</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2289</c:v>
+                  <c:v>0.0161</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.7841</c:v>
+                  <c:v>36.2692</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.0149</c:v>
+                  <c:v>49.6784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>67.8751</c:v>
+                  <c:v>71.2483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2066468224"/>
-        <c:axId val="-2065859184"/>
+        <c:axId val="-2093459520"/>
+        <c:axId val="-2093453264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2066468224"/>
+        <c:axId val="-2093459520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065859184"/>
+        <c:crossAx val="-2093453264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2065859184"/>
+        <c:axId val="-2093453264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066468224"/>
+        <c:crossAx val="-2093459520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3360,16 +3357,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3355</c:v>
+                    <c:v>0.3499</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.2321</c:v>
+                    <c:v>5.8325</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.2725</c:v>
+                    <c:v>3.2977</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.5986</c:v>
+                    <c:v>0.7103</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3384,16 +3381,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.0859</c:v>
+                    <c:v>1.1405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.729</c:v>
+                    <c:v>8.9604</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.4065</c:v>
+                    <c:v>5.5643</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7916</c:v>
+                    <c:v>4.9445</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3446,16 +3443,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0955</c:v>
+                  <c:v>23.041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.9385</c:v>
+                  <c:v>62.5123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.6066</c:v>
+                  <c:v>66.0897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.5922</c:v>
+                  <c:v>83.9853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3510,13 +3507,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.1254</c:v>
+                    <c:v>10.558</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.7082</c:v>
+                    <c:v>14.7853</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.005</c:v>
+                    <c:v>5.8573</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3534,13 +3531,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>14.7821</c:v>
+                    <c:v>17.1179</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.2387</c:v>
+                    <c:v>3.3596</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.3363</c:v>
+                    <c:v>5.0629</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3596,13 +3593,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.3372</c:v>
+                  <c:v>44.3952</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.8528</c:v>
+                  <c:v>43.8728</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66.929</c:v>
+                  <c:v>69.7166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,13 +3654,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.5077</c:v>
+                    <c:v>12.0595</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>18.0465</c:v>
+                    <c:v>11.4206</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3065</c:v>
+                    <c:v>3.3153</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3681,13 +3678,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>18.4389</c:v>
+                    <c:v>19.3686</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.0247</c:v>
+                    <c:v>5.846</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.6625</c:v>
+                    <c:v>3.5999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3743,13 +3740,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.3659</c:v>
+                  <c:v>23.4429</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.4054</c:v>
+                  <c:v>25.3587</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.5742</c:v>
+                  <c:v>50.2518</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3804,13 +3801,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.6281</c:v>
+                    <c:v>13.2249</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.692</c:v>
+                    <c:v>16.2897</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.146</c:v>
+                    <c:v>4.1034</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3828,13 +3825,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>18.1547</c:v>
+                    <c:v>21.0755</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.2058</c:v>
+                    <c:v>11.6614</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.3289</c:v>
+                    <c:v>0.7335</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3890,13 +3887,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.5686</c:v>
+                  <c:v>24.8547</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.9044</c:v>
+                  <c:v>26.3264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.7271</c:v>
+                  <c:v>50.8615</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079984352"/>
-        <c:axId val="-2137919376"/>
+        <c:axId val="-2093394496"/>
+        <c:axId val="-2093388240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079984352"/>
+        <c:axId val="-2093394496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137919376"/>
+        <c:crossAx val="-2093388240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2137919376"/>
+        <c:axId val="-2093388240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079984352"/>
+        <c:crossAx val="-2093394496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6606,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>22.500800000000002</v>
-          </cell>
-          <cell r="F4">
-            <v>0.37819999999999998</v>
-          </cell>
-          <cell r="G4">
-            <v>0.1023</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>34.633699999999997</v>
-          </cell>
-          <cell r="F5">
-            <v>0.19270000000000001</v>
-          </cell>
-          <cell r="G5">
-            <v>0.19239999999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>40.602200000000003</v>
-          </cell>
-          <cell r="F6">
-            <v>0.37769999999999998</v>
-          </cell>
-          <cell r="G6">
-            <v>0.43319999999999997</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>43.945</v>
-          </cell>
-          <cell r="F7">
-            <v>0.1847</v>
-          </cell>
-          <cell r="G7">
-            <v>0.3407</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>45.708100000000002</v>
-          </cell>
-          <cell r="F8">
-            <v>0.26390000000000002</v>
-          </cell>
-          <cell r="G8">
-            <v>0.15379999999999999</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>2.3784000000000001</v>
-          </cell>
-          <cell r="F10">
-            <v>0.74729999999999996</v>
-          </cell>
-          <cell r="G10">
-            <v>1.3210999999999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>25.444700000000001</v>
-          </cell>
-          <cell r="F11">
-            <v>0.28999999999999998</v>
-          </cell>
-          <cell r="G11">
-            <v>1.78E-2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>37.452800000000003</v>
-          </cell>
-          <cell r="F12">
-            <v>0.3715</v>
-          </cell>
-          <cell r="G12">
-            <v>0.13289999999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>43.572600000000001</v>
-          </cell>
-          <cell r="F13">
-            <v>0.46279999999999999</v>
-          </cell>
-          <cell r="G13">
-            <v>0.21640000000000001</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>46.484499999999997</v>
-          </cell>
-          <cell r="F14">
-            <v>0.13719999999999999</v>
-          </cell>
-          <cell r="G14">
-            <v>0.2636</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>2.63E-2</v>
-          </cell>
-          <cell r="F16">
-            <v>0.26050000000000001</v>
-          </cell>
-          <cell r="G16">
-            <v>0.1004</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>20.241800000000001</v>
-          </cell>
-          <cell r="F17">
-            <v>1.66E-2</v>
-          </cell>
-          <cell r="G17">
-            <v>1.46E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>33.987299999999998</v>
-          </cell>
-          <cell r="F18">
-            <v>2.5651999999999999</v>
-          </cell>
-          <cell r="G18">
-            <v>0.39610000000000001</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>41.860900000000001</v>
-          </cell>
-          <cell r="F19">
-            <v>8.6300000000000002E-2</v>
-          </cell>
-          <cell r="G19">
-            <v>0.13769999999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>45.838299999999997</v>
-          </cell>
-          <cell r="F20">
-            <v>0.31869999999999998</v>
-          </cell>
-          <cell r="G20">
-            <v>3.1600000000000003E-2</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>5.0599999999999999E-2</v>
-          </cell>
-          <cell r="F22">
-            <v>2.1700000000000001E-2</v>
-          </cell>
-          <cell r="G22">
-            <v>2.3999999999999998E-3</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>19.996300000000002</v>
-          </cell>
-          <cell r="F23">
-            <v>8.3400000000000002E-2</v>
-          </cell>
-          <cell r="G23">
-            <v>3.04E-2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>33.838799999999999</v>
-          </cell>
-          <cell r="F24">
-            <v>2.556</v>
-          </cell>
-          <cell r="G24">
-            <v>0.3785</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>41.792000000000002</v>
-          </cell>
-          <cell r="F25">
-            <v>0.68120000000000003</v>
-          </cell>
-          <cell r="G25">
-            <v>0.1255</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>45.8277</v>
-          </cell>
-          <cell r="F26">
-            <v>0.41439999999999999</v>
-          </cell>
-          <cell r="G26">
-            <v>3.09E-2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>26.218399999999999</v>
-          </cell>
-          <cell r="F29">
-            <v>3.0000000000000001E-3</v>
-          </cell>
-          <cell r="G29">
-            <v>8.0000000000000004E-4</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>39.337899999999998</v>
-          </cell>
-          <cell r="F30">
-            <v>2.9999999999999997E-4</v>
-          </cell>
-          <cell r="G30">
-            <v>5.9999999999999995E-4</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>46.2376</v>
-          </cell>
-          <cell r="F31">
-            <v>0.33760000000000001</v>
-          </cell>
-          <cell r="G31">
-            <v>0.29389999999999999</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>49.157699999999998</v>
-          </cell>
-          <cell r="F32">
-            <v>0.2656</v>
-          </cell>
-          <cell r="G32">
-            <v>0.82030000000000003</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>51.252099999999999</v>
-          </cell>
-          <cell r="F33">
-            <v>0.14319999999999999</v>
-          </cell>
-          <cell r="G33">
-            <v>0.17349999999999999</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>1.2829999999999999</v>
-          </cell>
-          <cell r="F35">
-            <v>1.8588</v>
-          </cell>
-          <cell r="G35">
-            <v>0.26079999999999998</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>25.184899999999999</v>
-          </cell>
-          <cell r="F36">
-            <v>0.1026</v>
-          </cell>
-          <cell r="G36">
-            <v>0.2908</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>37.589300000000001</v>
-          </cell>
-          <cell r="F37">
-            <v>0.20979999999999999</v>
-          </cell>
-          <cell r="G37">
-            <v>0.2999</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>43.793900000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>0.67589999999999995</v>
-          </cell>
-          <cell r="G38">
-            <v>0.7913</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>46.885399999999997</v>
-          </cell>
-          <cell r="F39">
-            <v>0.17399999999999999</v>
-          </cell>
-          <cell r="G39">
-            <v>6.0100000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>0</v>
-          </cell>
-          <cell r="F41">
-            <v>0</v>
-          </cell>
-          <cell r="G41">
-            <v>0.20749999999999999</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>10.542400000000001</v>
-          </cell>
-          <cell r="F42">
-            <v>1.3299999999999999E-2</v>
-          </cell>
-          <cell r="G42">
-            <v>0.1424</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>29.5395</v>
-          </cell>
-          <cell r="F43">
-            <v>8.9700000000000002E-2</v>
-          </cell>
-          <cell r="G43">
-            <v>1.0396000000000001</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>39.436399999999999</v>
-          </cell>
-          <cell r="F44">
-            <v>0.16339999999999999</v>
-          </cell>
-          <cell r="G44">
-            <v>0.1207</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>44.684600000000003</v>
-          </cell>
-          <cell r="F45">
-            <v>0.23669999999999999</v>
-          </cell>
-          <cell r="G45">
-            <v>0.57120000000000004</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>10.8195</v>
-          </cell>
-          <cell r="F48">
-            <v>0.12690000000000001</v>
-          </cell>
-          <cell r="G48">
-            <v>0.13669999999999999</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>29.665900000000001</v>
-          </cell>
-          <cell r="F49">
-            <v>0.2616</v>
-          </cell>
-          <cell r="G49">
-            <v>1.0583</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>39.319499999999998</v>
-          </cell>
-          <cell r="F50">
-            <v>0.50039999999999996</v>
-          </cell>
-          <cell r="G50">
-            <v>0.22919999999999999</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>44.971800000000002</v>
-          </cell>
-          <cell r="F51">
-            <v>0.51039999999999996</v>
-          </cell>
-          <cell r="G51">
-            <v>0.19270000000000001</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>48.340899999999998</v>
-          </cell>
-          <cell r="F54">
-            <v>0</v>
-          </cell>
-          <cell r="G54">
-            <v>0.38369999999999999</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>74.115499999999997</v>
-          </cell>
-          <cell r="F55">
-            <v>0.14380000000000001</v>
-          </cell>
-          <cell r="G55">
-            <v>4.87E-2</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>86.906499999999994</v>
-          </cell>
-          <cell r="F56">
-            <v>0.19900000000000001</v>
-          </cell>
-          <cell r="G56">
-            <v>7.5999999999999998E-2</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>93.337400000000002</v>
-          </cell>
-          <cell r="F57">
-            <v>7.2099999999999997E-2</v>
-          </cell>
-          <cell r="G57">
-            <v>0.1202</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>96.683499999999995</v>
-          </cell>
-          <cell r="F58">
-            <v>6.3700000000000007E-2</v>
-          </cell>
-          <cell r="G58">
-            <v>2.4299999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>3.93</v>
-          </cell>
-          <cell r="F60">
-            <v>1.4035</v>
-          </cell>
-          <cell r="G60">
-            <v>0.65069999999999995</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>50.531700000000001</v>
-          </cell>
-          <cell r="F61">
-            <v>0.19239999999999999</v>
-          </cell>
-          <cell r="G61">
-            <v>1.67E-2</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>75.118600000000001</v>
-          </cell>
-          <cell r="F62">
-            <v>0.14760000000000001</v>
-          </cell>
-          <cell r="G62">
-            <v>5.6500000000000002E-2</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>87.535300000000007</v>
-          </cell>
-          <cell r="F63">
-            <v>0.1016</v>
-          </cell>
-          <cell r="G63">
-            <v>4.7699999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>93.741900000000001</v>
-          </cell>
-          <cell r="F64">
-            <v>1.4800000000000001E-2</v>
-          </cell>
-          <cell r="G64">
-            <v>3.0800000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>0.12670000000000001</v>
-          </cell>
-          <cell r="F66">
-            <v>2.3900000000000001E-2</v>
-          </cell>
-          <cell r="G66">
-            <v>0.2072</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>30.785799999999998</v>
-          </cell>
-          <cell r="F67">
-            <v>1.66E-2</v>
-          </cell>
-          <cell r="G67">
-            <v>1.77E-2</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>63.492699999999999</v>
-          </cell>
-          <cell r="F68">
-            <v>1.4125000000000001</v>
-          </cell>
-          <cell r="G68">
-            <v>0.2167</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>81.367099999999994</v>
-          </cell>
-          <cell r="F69">
-            <v>2.8000000000000001E-2</v>
-          </cell>
-          <cell r="G69">
-            <v>3.78E-2</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>90.533900000000003</v>
-          </cell>
-          <cell r="F70">
-            <v>6.83E-2</v>
-          </cell>
-          <cell r="G70">
-            <v>3.9600000000000003E-2</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>5.0599999999999999E-2</v>
-          </cell>
-          <cell r="F72">
-            <v>1.9300000000000001E-2</v>
-          </cell>
-          <cell r="G72">
-            <v>2.3999999999999998E-3</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>30.817299999999999</v>
-          </cell>
-          <cell r="F73">
-            <v>6.9900000000000004E-2</v>
-          </cell>
-          <cell r="G73">
-            <v>2.8899999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>63.491</v>
-          </cell>
-          <cell r="F74">
-            <v>1.4072</v>
-          </cell>
-          <cell r="G74">
-            <v>0.2049</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>81.3613</v>
-          </cell>
-          <cell r="F75">
-            <v>0.2167</v>
-          </cell>
-          <cell r="G75">
-            <v>4.4600000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>90.574100000000001</v>
-          </cell>
-          <cell r="F76">
-            <v>6.6500000000000004E-2</v>
-          </cell>
-          <cell r="G76">
-            <v>5.1000000000000004E-3</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>29.983799999999999</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0.51919999999999999</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>57.330199999999998</v>
-          </cell>
-          <cell r="F80">
-            <v>0.23730000000000001</v>
-          </cell>
-          <cell r="G80">
-            <v>8.0399999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>75.679299999999998</v>
-          </cell>
-          <cell r="F81">
-            <v>0.53979999999999995</v>
-          </cell>
-          <cell r="G81">
-            <v>0.25130000000000002</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>86.895499999999998</v>
-          </cell>
-          <cell r="F82">
-            <v>0.35909999999999997</v>
-          </cell>
-          <cell r="G82">
-            <v>0.22570000000000001</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>93.188699999999997</v>
-          </cell>
-          <cell r="F83">
-            <v>0.10249999999999999</v>
-          </cell>
-          <cell r="G83">
-            <v>6.59E-2</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>3.0844999999999998</v>
-          </cell>
-          <cell r="F85">
-            <v>0.40310000000000001</v>
-          </cell>
-          <cell r="G85">
-            <v>4.5999999999999999E-3</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>33.653300000000002</v>
-          </cell>
-          <cell r="F86">
-            <v>3.2000000000000001E-2</v>
-          </cell>
-          <cell r="G86">
-            <v>0.33879999999999999</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>60.084699999999998</v>
-          </cell>
-          <cell r="F87">
-            <v>0.38190000000000002</v>
-          </cell>
-          <cell r="G87">
-            <v>0.1386</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>77.902699999999996</v>
-          </cell>
-          <cell r="F88">
-            <v>0.31</v>
-          </cell>
-          <cell r="G88">
-            <v>5.4000000000000003E-3</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>88.226399999999998</v>
-          </cell>
-          <cell r="F89">
-            <v>3.9699999999999999E-2</v>
-          </cell>
-          <cell r="G89">
-            <v>4.9399999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0.12670000000000001</v>
-          </cell>
-          <cell r="F91">
-            <v>2.3900000000000001E-2</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>22.640499999999999</v>
-          </cell>
-          <cell r="F92">
-            <v>0.15329999999999999</v>
-          </cell>
-          <cell r="G92">
-            <v>4.1999999999999997E-3</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>48.213299999999997</v>
-          </cell>
-          <cell r="F93">
-            <v>2.8363999999999998</v>
-          </cell>
-          <cell r="G93">
-            <v>0.28179999999999999</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>69.235200000000006</v>
-          </cell>
-          <cell r="F94">
-            <v>4.9099999999999998E-2</v>
-          </cell>
-          <cell r="G94">
-            <v>8.1699999999999995E-2</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>82.854200000000006</v>
-          </cell>
-          <cell r="F95">
-            <v>8.3099999999999993E-2</v>
-          </cell>
-          <cell r="G95">
-            <v>0.10580000000000001</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>5.0599999999999999E-2</v>
-          </cell>
-          <cell r="F97">
-            <v>1.9300000000000001E-2</v>
-          </cell>
-          <cell r="G97">
-            <v>2.3999999999999998E-3</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>22.435700000000001</v>
-          </cell>
-          <cell r="F98">
-            <v>9.8400000000000001E-2</v>
-          </cell>
-          <cell r="G98">
-            <v>2.0199999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>48.047499999999999</v>
-          </cell>
-          <cell r="F99">
-            <v>2.7797000000000001</v>
-          </cell>
-          <cell r="G99">
-            <v>0.5272</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>69.248400000000004</v>
-          </cell>
-          <cell r="F100">
-            <v>6.7500000000000004E-2</v>
-          </cell>
-          <cell r="G100">
-            <v>4.2999999999999997E-2</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>82.874700000000004</v>
-          </cell>
-          <cell r="F101">
-            <v>6.4000000000000001E-2</v>
-          </cell>
-          <cell r="G101">
-            <v>3.39E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7786,7 +6874,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7850,13 +6938,13 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-1.03E-2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1.03E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7873,13 +6961,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>17.238099999999999</v>
+        <v>16.805700000000002</v>
       </c>
       <c r="F5">
-        <v>0.85809999999999997</v>
+        <v>0.82169999999999999</v>
       </c>
       <c r="G5">
-        <v>0.26169999999999999</v>
+        <v>0.26369999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7902,7 +6990,7 @@
         <v>5.5888</v>
       </c>
       <c r="G6">
-        <v>3.5430000000000001</v>
+        <v>3.508</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7007,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>37.366900000000001</v>
+        <v>37.019399999999997</v>
       </c>
       <c r="F7">
-        <v>0.45179999999999998</v>
+        <v>0.7329</v>
       </c>
       <c r="G7">
-        <v>3.6985999999999999</v>
+        <v>2.7845</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7030,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>43.737499999999997</v>
+        <v>43.437800000000003</v>
       </c>
       <c r="F8">
-        <v>0.55379999999999996</v>
+        <v>0.23549999999999999</v>
       </c>
       <c r="G8">
-        <v>0.62960000000000005</v>
+        <v>1.4554</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7965,13 +7053,13 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>-0.17180000000000001</v>
       </c>
       <c r="F10">
-        <v>0.14960000000000001</v>
+        <v>0.52339999999999998</v>
       </c>
       <c r="G10">
-        <v>0.1321</v>
+        <v>0.5806</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7122,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>25.740200000000002</v>
+        <v>27.286899999999999</v>
       </c>
       <c r="F13">
-        <v>6.4233000000000002</v>
+        <v>2.6385000000000001</v>
       </c>
       <c r="G13">
-        <v>8.2149999999999999</v>
+        <v>6.7496999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7145,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>38.281599999999997</v>
+        <v>37.775799999999997</v>
       </c>
       <c r="F14">
-        <v>4.1418999999999997</v>
+        <v>2.9095</v>
       </c>
       <c r="G14">
-        <v>3.6036999999999999</v>
+        <v>3.8679000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8080,13 +7168,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>-9.1700000000000004E-2</v>
       </c>
       <c r="F16">
-        <v>5.67E-2</v>
+        <v>9.2499999999999999E-2</v>
       </c>
       <c r="G16">
-        <v>5.5399999999999998E-2</v>
+        <v>0.27579999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -8103,13 +7191,13 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.192</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.79469999999999996</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>0.68179999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8126,13 +7214,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>21.405999999999999</v>
+        <v>20.079000000000001</v>
       </c>
       <c r="F18">
-        <v>17.685300000000002</v>
+        <v>16.3748</v>
       </c>
       <c r="G18">
-        <v>11.0158</v>
+        <v>10.3392</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7237,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>11.6884</v>
+        <v>14.351100000000001</v>
       </c>
       <c r="F19">
-        <v>1.7146999999999999</v>
+        <v>2.9020999999999999</v>
       </c>
       <c r="G19">
-        <v>13.567500000000001</v>
+        <v>5.0260999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7260,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>30.694099999999999</v>
+        <v>29.5063</v>
       </c>
       <c r="F20">
-        <v>1.4945999999999999</v>
+        <v>4.3337000000000003</v>
       </c>
       <c r="G20">
-        <v>0.9889</v>
+        <v>6.1886999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8195,13 +7283,13 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.33160000000000001</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1.109</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>0.32940000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -8218,13 +7306,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>-0.24410000000000001</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1.4681</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1.9749000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -8247,7 +7335,7 @@
         <v>17.539000000000001</v>
       </c>
       <c r="G24">
-        <v>11.4734</v>
+        <v>11.4017</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -8264,13 +7352,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>11.173999999999999</v>
+        <v>14.4742</v>
       </c>
       <c r="F25">
-        <v>1.6026</v>
+        <v>2.9285999999999999</v>
       </c>
       <c r="G25">
-        <v>15.063000000000001</v>
+        <v>19.715699999999998</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7375,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>30.448599999999999</v>
+        <v>30.1845</v>
       </c>
       <c r="F26">
-        <v>1.0718000000000001</v>
+        <v>1.0716000000000001</v>
       </c>
       <c r="G26">
-        <v>1.0788</v>
+        <v>7.0030999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8318,13 +7406,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>-3.8346</v>
+        <v>10.907400000000001</v>
       </c>
       <c r="F29">
-        <v>0.52749999999999997</v>
+        <v>0.2828</v>
       </c>
       <c r="G29">
-        <v>0.10730000000000001</v>
+        <v>1.3125</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -8341,13 +7429,13 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>21.983799999999999</v>
+        <v>27.025200000000002</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>1.04E-2</v>
+        <v>2.92E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -8364,10 +7452,10 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>35.973199999999999</v>
+        <v>37.578200000000002</v>
       </c>
       <c r="F31">
-        <v>1.41E-2</v>
+        <v>1.04E-2</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -8387,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>43.386400000000002</v>
+        <v>43.547899999999998</v>
       </c>
       <c r="F32">
-        <v>1.0591999999999999</v>
+        <v>0.188</v>
       </c>
       <c r="G32">
-        <v>0.31219999999999998</v>
+        <v>0.9778</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7498,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>46.470100000000002</v>
+        <v>46.825000000000003</v>
       </c>
       <c r="F33">
-        <v>0.31119999999999998</v>
+        <v>0.1492</v>
       </c>
       <c r="G33">
-        <v>0.73719999999999997</v>
+        <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7521,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>0.66649999999999998</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>6.0900000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>7.1099999999999997E-2</v>
+        <v>1.0181</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8456,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>-3.3066</v>
+        <v>15.2135</v>
       </c>
       <c r="F36">
-        <v>1.4800000000000001E-2</v>
+        <v>0.20030000000000001</v>
       </c>
       <c r="G36">
-        <v>4.3499999999999997E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8479,10 +7567,10 @@
         <v>8</v>
       </c>
       <c r="E37">
-        <v>23.038799999999998</v>
+        <v>33.540700000000001</v>
       </c>
       <c r="F37">
-        <v>1.9400000000000001E-2</v>
+        <v>2.81E-2</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -8502,13 +7590,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>36.491900000000001</v>
+        <v>41.751899999999999</v>
       </c>
       <c r="F38">
-        <v>0.39829999999999999</v>
+        <v>0.1845</v>
       </c>
       <c r="G38">
-        <v>4.1999999999999997E-3</v>
+        <v>1.2954000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7613,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>43.240400000000001</v>
+        <v>45.872599999999998</v>
       </c>
       <c r="F39">
-        <v>0.32119999999999999</v>
+        <v>0.10630000000000001</v>
       </c>
       <c r="G39">
-        <v>0.2445</v>
+        <v>0.44840000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8548,13 +7636,13 @@
         <v>2</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>2.24E-2</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>0.126</v>
       </c>
       <c r="G41">
-        <v>5.5399999999999998E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8571,13 +7659,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>-25.8263</v>
+        <v>0.8075</v>
       </c>
       <c r="F42">
-        <v>0.14069999999999999</v>
+        <v>0.29520000000000002</v>
       </c>
       <c r="G42">
-        <v>0.41310000000000002</v>
+        <v>0.95489999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -8594,13 +7682,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>4.2622999999999998</v>
+        <v>14.321</v>
       </c>
       <c r="F43">
-        <v>6.3799999999999996E-2</v>
+        <v>0.1996</v>
       </c>
       <c r="G43">
-        <v>2.9399999999999999E-2</v>
+        <v>0.20030000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7705,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>26.016400000000001</v>
+        <v>28.476800000000001</v>
       </c>
       <c r="F44">
-        <v>0.78810000000000002</v>
+        <v>0.98529999999999995</v>
       </c>
       <c r="G44">
-        <v>1.8937999999999999</v>
+        <v>0.10150000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7728,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>38.520299999999999</v>
+        <v>39.173299999999998</v>
       </c>
       <c r="F45">
-        <v>1.2095</v>
+        <v>1.9031</v>
       </c>
       <c r="G45">
-        <v>1.2844</v>
+        <v>2.2766000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8663,13 +7751,13 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>0.15909999999999999</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>0.59730000000000005</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>0.26169999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -8686,13 +7774,13 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>3.2288999999999999</v>
+        <v>1.61E-2</v>
       </c>
       <c r="F48">
-        <v>3.9399999999999998E-2</v>
+        <v>0.87219999999999998</v>
       </c>
       <c r="G48">
-        <v>1.34E-2</v>
+        <v>1.2133</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7797,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>2.8248000000000002</v>
+        <v>15.3652</v>
       </c>
       <c r="F49">
-        <v>1.72E-2</v>
+        <v>0.2185</v>
       </c>
       <c r="G49">
-        <v>0.2344</v>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7820,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>25.581399999999999</v>
+        <v>31.973800000000001</v>
       </c>
       <c r="F50">
-        <v>0.81010000000000004</v>
+        <v>0.53559999999999997</v>
       </c>
       <c r="G50">
-        <v>2.3727999999999998</v>
+        <v>2.1941000000000002</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7843,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>37.437899999999999</v>
+        <v>41.106000000000002</v>
       </c>
       <c r="F51">
-        <v>0.39140000000000003</v>
+        <v>0.95279999999999998</v>
       </c>
       <c r="G51">
-        <v>0.64049999999999996</v>
+        <v>1.8188</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7874,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>-3.8346</v>
+        <v>10.907400000000001</v>
       </c>
       <c r="F54">
-        <v>0.52749999999999997</v>
+        <v>0.2828</v>
       </c>
       <c r="G54">
-        <v>0.10730000000000001</v>
+        <v>1.3125</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7897,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>39.221800000000002</v>
+        <v>43.839300000000001</v>
       </c>
       <c r="F55">
-        <v>0.83879999999999999</v>
+        <v>0.80940000000000001</v>
       </c>
       <c r="G55">
-        <v>0.26179999999999998</v>
+        <v>0.25530000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7920,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>74.990200000000002</v>
+        <v>76.599500000000006</v>
       </c>
       <c r="F56">
-        <v>5.5888999999999998</v>
+        <v>5.5932000000000004</v>
       </c>
       <c r="G56">
-        <v>3.3452000000000002</v>
+        <v>3.6374</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7943,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>81.661600000000007</v>
+        <v>80.933099999999996</v>
       </c>
       <c r="F57">
-        <v>1.395</v>
+        <v>3.1307999999999998</v>
       </c>
       <c r="G57">
-        <v>2.9843000000000002</v>
+        <v>2.0847000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7966,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>90.127700000000004</v>
+        <v>91.467799999999997</v>
       </c>
       <c r="F58">
-        <v>0.27150000000000002</v>
+        <v>2.6128999999999998</v>
       </c>
       <c r="G58">
-        <v>0.8458</v>
+        <v>0.44729999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7989,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>0.66649999999999998</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>6.0900000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>7.1099999999999997E-2</v>
+        <v>1.0181</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8924,13 +8012,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>-3.3066</v>
+        <v>15.2135</v>
       </c>
       <c r="F61">
-        <v>1.4800000000000001E-2</v>
+        <v>0.20030000000000001</v>
       </c>
       <c r="G61">
-        <v>4.3499999999999997E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8035,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>52.543500000000002</v>
+        <v>63.045499999999997</v>
       </c>
       <c r="F62">
-        <v>11.3764</v>
+        <v>11.3765</v>
       </c>
       <c r="G62">
-        <v>7.0129000000000001</v>
+        <v>7.0041000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8058,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>64.343500000000006</v>
+        <v>67.299499999999995</v>
       </c>
       <c r="F63">
-        <v>3.3269000000000002</v>
+        <v>1.1789000000000001</v>
       </c>
       <c r="G63">
-        <v>2.9885999999999999</v>
+        <v>8.6196000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8081,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>81.229100000000003</v>
+        <v>83.5762</v>
       </c>
       <c r="F64">
-        <v>0.6744</v>
+        <v>2.7075</v>
       </c>
       <c r="G64">
-        <v>1.0382</v>
+        <v>3.2631000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9016,13 +8104,13 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>2.24E-2</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>0.126</v>
       </c>
       <c r="G66">
-        <v>5.5399999999999998E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9039,13 +8127,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>-25.8263</v>
+        <v>0.8075</v>
       </c>
       <c r="F67">
-        <v>0.14069999999999999</v>
+        <v>0.29520000000000002</v>
       </c>
       <c r="G67">
-        <v>0.41310000000000002</v>
+        <v>0.95489999999999997</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8150,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>25.697700000000001</v>
+        <v>34.4283</v>
       </c>
       <c r="F68">
-        <v>17.690899999999999</v>
+        <v>16.424399999999999</v>
       </c>
       <c r="G68">
-        <v>11.010199999999999</v>
+        <v>10.3108</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8173,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>38.745600000000003</v>
+        <v>45.953299999999999</v>
       </c>
       <c r="F69">
-        <v>2.1747999999999998</v>
+        <v>4.2923999999999998</v>
       </c>
       <c r="G69">
-        <v>12.9907</v>
+        <v>8.8292000000000002</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8196,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>68.383600000000001</v>
+        <v>69.575000000000003</v>
       </c>
       <c r="F70">
-        <v>0.80510000000000004</v>
+        <v>0.81030000000000002</v>
       </c>
       <c r="G70">
-        <v>0.6915</v>
+        <v>1.5918000000000001</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9131,13 +8219,13 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>0.15909999999999999</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>0.59730000000000005</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>0.26169999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9154,13 +8242,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>3.2288999999999999</v>
+        <v>1.61E-2</v>
       </c>
       <c r="F73">
-        <v>3.9399999999999998E-2</v>
+        <v>0.87219999999999998</v>
       </c>
       <c r="G73">
-        <v>1.34E-2</v>
+        <v>1.2133</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8265,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>23.784099999999999</v>
+        <v>36.269199999999998</v>
       </c>
       <c r="F74">
-        <v>17.5532</v>
+        <v>17.616099999999999</v>
       </c>
       <c r="G74">
-        <v>11.456300000000001</v>
+        <v>11.3246</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8288,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>43.014899999999997</v>
+        <v>49.678400000000003</v>
       </c>
       <c r="F75">
-        <v>7.9104000000000001</v>
+        <v>8.1856000000000009</v>
       </c>
       <c r="G75">
-        <v>7.6696</v>
+        <v>11.2408</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8311,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>67.875100000000003</v>
+        <v>71.2483</v>
       </c>
       <c r="F76">
-        <v>4.5377000000000001</v>
+        <v>0.83440000000000003</v>
       </c>
       <c r="G76">
-        <v>2.0217000000000001</v>
+        <v>2.2286999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9274,13 +8362,13 @@
         <v>4</v>
       </c>
       <c r="E80">
-        <v>22.095500000000001</v>
+        <v>23.041</v>
       </c>
       <c r="F80">
-        <v>1.0859000000000001</v>
+        <v>1.1405000000000001</v>
       </c>
       <c r="G80">
-        <v>0.33550000000000002</v>
+        <v>0.34989999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,13 +8385,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>60.938499999999998</v>
+        <v>62.512300000000003</v>
       </c>
       <c r="F81">
-        <v>8.7289999999999992</v>
+        <v>8.9603999999999999</v>
       </c>
       <c r="G81">
-        <v>5.2321</v>
+        <v>5.8324999999999996</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8408,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>67.6066</v>
+        <v>66.089699999999993</v>
       </c>
       <c r="F82">
-        <v>2.4064999999999999</v>
+        <v>5.5643000000000002</v>
       </c>
       <c r="G82">
-        <v>5.2725</v>
+        <v>3.2976999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8431,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>81.592200000000005</v>
+        <v>83.985299999999995</v>
       </c>
       <c r="F83">
-        <v>0.79159999999999997</v>
+        <v>4.9444999999999997</v>
       </c>
       <c r="G83">
-        <v>1.5986</v>
+        <v>0.71030000000000004</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9412,13 +8500,13 @@
         <v>8</v>
       </c>
       <c r="E87">
-        <v>38.337200000000003</v>
+        <v>44.395200000000003</v>
       </c>
       <c r="F87">
-        <v>14.7821</v>
+        <v>17.117899999999999</v>
       </c>
       <c r="G87">
-        <v>9.1254000000000008</v>
+        <v>10.558</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8523,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>43.852800000000002</v>
+        <v>43.872799999999998</v>
       </c>
       <c r="F88">
-        <v>5.2386999999999997</v>
+        <v>3.3595999999999999</v>
       </c>
       <c r="G88">
-        <v>4.7081999999999997</v>
+        <v>14.785299999999999</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8546,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>66.929000000000002</v>
+        <v>69.7166</v>
       </c>
       <c r="F89">
-        <v>1.3363</v>
+        <v>5.0629</v>
       </c>
       <c r="G89">
-        <v>2.0049999999999999</v>
+        <v>5.8573000000000004</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9527,13 +8615,13 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <v>22.3659</v>
+        <v>23.442900000000002</v>
       </c>
       <c r="F93">
-        <v>18.4389</v>
+        <v>19.368600000000001</v>
       </c>
       <c r="G93">
-        <v>11.5077</v>
+        <v>12.0595</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8638,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>17.4054</v>
+        <v>25.358699999999999</v>
       </c>
       <c r="F94">
-        <v>4.0247000000000002</v>
+        <v>5.8460000000000001</v>
       </c>
       <c r="G94">
-        <v>18.046500000000002</v>
+        <v>11.4206</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8661,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>48.574199999999998</v>
+        <v>50.251800000000003</v>
       </c>
       <c r="F95">
-        <v>1.6625000000000001</v>
+        <v>3.5998999999999999</v>
       </c>
       <c r="G95">
-        <v>0.30649999999999999</v>
+        <v>3.3153000000000001</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9642,13 +8730,13 @@
         <v>8</v>
       </c>
       <c r="E99">
-        <v>21.5686</v>
+        <v>24.854700000000001</v>
       </c>
       <c r="F99">
-        <v>18.154699999999998</v>
+        <v>21.075500000000002</v>
       </c>
       <c r="G99">
-        <v>11.6281</v>
+        <v>13.2249</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8753,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>20.904399999999999</v>
+        <v>26.3264</v>
       </c>
       <c r="F100">
-        <v>8.2058</v>
+        <v>11.6614</v>
       </c>
       <c r="G100">
-        <v>12.692</v>
+        <v>16.2897</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8776,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>48.7271</v>
+        <v>50.861499999999999</v>
       </c>
       <c r="F101">
-        <v>7.3289</v>
+        <v>0.73350000000000004</v>
       </c>
       <c r="G101">
-        <v>3.1459999999999999</v>
+        <v>4.1033999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix dip in graph
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_uneven_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_uneven_striping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -252,7 +249,7 @@
                   <c:v>39.0169</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.0194</c:v>
+                  <c:v>39.79</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43.4378</c:v>
@@ -329,7 +326,7 @@
                   <c:v>29.5048</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.2869</c:v>
+                  <c:v>33.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>37.7758</c:v>
@@ -406,7 +403,7 @@
                   <c:v>20.079</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.3511</c:v>
+                  <c:v>20.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>29.5063</c:v>
@@ -483,7 +480,7 @@
                   <c:v>20.9594</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.4742</c:v>
+                  <c:v>22.168</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>30.1845</c:v>
@@ -501,11 +498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2005043488"/>
-        <c:axId val="-2005039184"/>
+        <c:axId val="-2115635904"/>
+        <c:axId val="-2114846528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2005043488"/>
+        <c:axId val="-2115635904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -621,12 +618,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005039184"/>
+        <c:crossAx val="-2114846528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2005039184"/>
+        <c:axId val="-2114846528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45.0"/>
@@ -749,7 +746,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005043488"/>
+        <c:crossAx val="-2115635904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1174,11 +1171,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2034182592"/>
-        <c:axId val="-2005902128"/>
+        <c:axId val="-2114627712"/>
+        <c:axId val="-2114621584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2034182592"/>
+        <c:axId val="-2114627712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -1294,12 +1291,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005902128"/>
+        <c:crossAx val="-2114621584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2005902128"/>
+        <c:axId val="-2114621584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60.0"/>
@@ -1415,7 +1412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2034182592"/>
+        <c:crossAx val="-2114627712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
@@ -1841,11 +1838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2004987200"/>
-        <c:axId val="-2033370944"/>
+        <c:axId val="-2114572688"/>
+        <c:axId val="-2114566560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2004987200"/>
+        <c:axId val="-2114572688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -1897,6 +1894,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1960,12 +1958,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2033370944"/>
+        <c:crossAx val="-2114566560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2033370944"/>
+        <c:axId val="-2114566560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2025,6 +2023,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2088,7 +2087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2004987200"/>
+        <c:crossAx val="-2114572688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2513,11 +2512,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2033441360"/>
-        <c:axId val="-2005759328"/>
+        <c:axId val="-2114517856"/>
+        <c:axId val="-2114511728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2033441360"/>
+        <c:axId val="-2114517856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -2569,6 +2568,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2632,12 +2632,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005759328"/>
+        <c:crossAx val="-2114511728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2005759328"/>
+        <c:axId val="-2114511728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2688,6 +2688,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2751,7 +2752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2033441360"/>
+        <c:crossAx val="-2114517856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5188,435 +5189,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>-1.03E-2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>16.805700000000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>39.0169</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>37.019399999999997</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>43.437800000000003</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>-0.17180000000000001</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>29.504799999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>27.286899999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>37.775799999999997</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>-9.1700000000000004E-2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0.192</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>20.079000000000001</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>14.351100000000001</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>29.5063</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0.33160000000000001</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>-0.24410000000000001</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>20.959399999999999</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>14.4742</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>30.1845</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>10.907400000000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>27.025200000000002</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>37.578200000000002</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>43.547899999999998</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>46.825000000000003</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>15.2135</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>33.540700000000001</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>41.751899999999999</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>45.872599999999998</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>2.24E-2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>0.8075</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>14.321</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>28.476800000000001</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>39.173299999999998</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0.15909999999999999</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>1.61E-2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>15.3652</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>31.973800000000001</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>41.106000000000002</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>10.907400000000001</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>43.839300000000001</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>76.599500000000006</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>80.933099999999996</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>91.467799999999997</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>15.2135</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>63.045499999999997</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>67.299499999999995</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>83.5762</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>2.24E-2</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>0.8075</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>34.4283</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>45.953299999999999</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>69.575000000000003</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0.15909999999999999</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>1.61E-2</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>36.269199999999998</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>49.678400000000003</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>71.2483</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>23.041</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>62.512300000000003</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>66.089699999999993</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>83.985299999999995</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>44.395200000000003</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>43.872799999999998</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>69.7166</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>23.442900000000002</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>25.358699999999999</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>50.251800000000003</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>24.854700000000001</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>26.3264</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>50.861499999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5882,8 +5454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L83" sqref="L83"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6019,7 +5591,7 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>37.019399999999997</v>
+        <v>39.79</v>
       </c>
       <c r="F7">
         <v>0.7329</v>
@@ -6134,7 +5706,7 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>27.286899999999999</v>
+        <v>33.9</v>
       </c>
       <c r="F13">
         <v>2.6385000000000001</v>
@@ -6249,7 +5821,7 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>14.351100000000001</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F19">
         <v>2.9020999999999999</v>
@@ -6364,7 +5936,7 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>14.4742</v>
+        <v>22.167999999999999</v>
       </c>
       <c r="F25">
         <v>2.9285999999999999</v>

</xml_diff>